<commit_message>
Define maybe condition in Entity diagram
</commit_message>
<xml_diff>
--- a/Sprint One/Entity Diagram.xlsx
+++ b/Sprint One/Entity Diagram.xlsx
@@ -66,13 +66,13 @@
     <t>Player.ID</t>
   </si>
   <si>
-    <t>-1,0,1</t>
-  </si>
-  <si>
     <t>Condition.ID</t>
   </si>
   <si>
     <t>Int</t>
+  </si>
+  <si>
+    <t>no, unknown, maybe, yes</t>
   </si>
 </sst>
 </file>
@@ -134,10 +134,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +445,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,22 +456,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -555,16 +555,16 @@
       <c r="J5" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>16</v>
+      <c r="K5" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" t="s">
         <v>17</v>
-      </c>
-      <c r="K6" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>